<commit_message>
ajout du plan d'acceptation
</commit_message>
<xml_diff>
--- a/Schmitt_Guillaume_2_plan_test_112022.xlsx
+++ b/Schmitt_Guillaume_2_plan_test_112022.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
   <si>
     <t xml:space="preserve">Fonctionnalité</t>
   </si>
@@ -37,34 +37,16 @@
     <t xml:space="preserve">Une page d’accueil montrant (de manière dynamique) tous les articles disponibles à la vente.</t>
   </si>
   <si>
-    <t xml:space="preserve">Ouvrir sur la page d'accueil du site web dans un navigateur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Affichage de l'ensemble des produits</t>
+    <t xml:space="preserve">Ouvrir sur la page d’accueil du site web dans un navigateur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Affichage de l’ensemble des produits</t>
   </si>
   <si>
     <t xml:space="preserve">OK </t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Montserrat"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">être rediriger vers la page du produit </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Montserrat"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">sélectionner sur la page d’accueil</t>
-    </r>
+    <t xml:space="preserve">être rediriger vers la page du produit sélectionner sur la page d’accueil</t>
   </si>
   <si>
     <t xml:space="preserve">sélectionner un produit sur la page d’accueil</t>
@@ -121,7 +103,7 @@
     <t xml:space="preserve">Ouvrir sur la page panier du site web dans un navigateur</t>
   </si>
   <si>
-    <t xml:space="preserve">Affichage de l'ensemble des produits du panier et du prix</t>
+    <t xml:space="preserve">Affichage de l’ensemble des produits du panier et du prix</t>
   </si>
   <si>
     <t xml:space="preserve">pouvoir supprimer un produit </t>
@@ -136,6 +118,9 @@
     <t xml:space="preserve">pouvoir modifier la quantité d’un produit </t>
   </si>
   <si>
+    <t xml:space="preserve">rajouter ou diminuer la quantité du produit  </t>
+  </si>
+  <si>
     <t xml:space="preserve">modification de la quantité du produit sélectionner sur la page sur le local storage et modification du prix total dynamiquement</t>
   </si>
   <si>
@@ -143,21 +128,40 @@
   </si>
   <si>
     <t xml:space="preserve">affichage dynamique du prix total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gestion des formulaire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">remplir le formulaire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pouvoir gérer les erreur de champs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">passer commande </t>
+  </si>
+  <si>
+    <t xml:space="preserve">cliquer sur «Commander ! »</t>
+  </si>
+  <si>
+    <t xml:space="preserve">passer commande, vider le local storage, générer un numéros de commande et être rediriger vers la page de confirmation </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="#,##0"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="6">
     <font>
-      <sz val="10"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -180,27 +184,15 @@
       <sz val="18"/>
       <color rgb="FF000000"/>
       <name val="Montserrat"/>
-      <family val="0"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Montserrat"/>
-      <family val="0"/>
+      <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <name val="Montserrat"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Montserrat"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="3">
@@ -213,7 +205,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD9D9D9"/>
-        <bgColor rgb="FFC0C0C0"/>
+        <bgColor rgb="FFC6C6C6"/>
       </patternFill>
     </fill>
   </fills>
@@ -226,31 +218,63 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="medium"/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="thin"/>
-      <top style="medium"/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="medium"/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom style="medium"/>
+      <left style="medium">
+        <color rgb="FFD9D9D9"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFD9D9D9"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFD9D9D9"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFD9D9D9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FFC6C6C6"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFD9D9D9"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFD9D9D9"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFD9D9D9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FFD9D9D9"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFD9D9D9"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFD9D9D9"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFD9D9D9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FFD9D9D9"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFD9D9D9"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFD9D9D9"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFD9D9D9"/>
+      </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -363,13 +387,25 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -381,14 +417,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -397,18 +433,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -416,48 +448,32 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -485,7 +501,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FFC6C6C6"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -539,289 +555,313 @@
   </sheetPr>
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.43359375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="19.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="58.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="57.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="52.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="2" width="58.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="57.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="52.72"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+    <row r="1" customFormat="false" ht="31.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4"/>
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="50.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="n">
+    <row r="2" customFormat="false" ht="54.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="n">
+      <c r="E2" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="38.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="12" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9" t="n">
+      <c r="E3" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="38.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="12" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="14" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9" t="n">
+      <c r="E4" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="38.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="12" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9" t="n">
+      <c r="E5" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="38.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="12" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9" t="n">
+      <c r="E6" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="23" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="12" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="9" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" s="15" t="s">
+      <c r="E7" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="23" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="12" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="9" t="n">
+      <c r="E8" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="38.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="12" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="50.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="9" t="n">
+      <c r="E9" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="54.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="12" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="67.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="9" t="n">
+      <c r="E10" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="54.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="12" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12" t="s">
+      <c r="C11" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="9" t="n">
+      <c r="D11" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="34.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="12" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="12" t="s">
+      <c r="B12" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="E12" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="9"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="18"/>
-    </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="19"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="18"/>
-    </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="19"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="18"/>
-    </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="19"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="18"/>
-    </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="19"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="18"/>
-    </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="19"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="18"/>
-    </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="19"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="18"/>
-    </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="19"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="18"/>
-    </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="19"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="18"/>
-    </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="20"/>
-      <c r="B22" s="21"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="23"/>
+      <c r="C12" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="23" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="12" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="15" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="23" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="15"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="16"/>
+    </row>
+    <row r="16" customFormat="false" ht="23" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="17"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="16"/>
+    </row>
+    <row r="17" customFormat="false" ht="23" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="17"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="16"/>
+    </row>
+    <row r="18" customFormat="false" ht="23" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="17"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="16"/>
+    </row>
+    <row r="19" customFormat="false" ht="23" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="17"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="16"/>
+    </row>
+    <row r="20" customFormat="false" ht="23" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="17"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="16"/>
+    </row>
+    <row r="21" customFormat="false" ht="23" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="17"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="16"/>
+    </row>
+    <row r="22" customFormat="false" ht="23" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="18"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="21"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>

</xml_diff>